<commit_message>
modified file belajar excel
</commit_message>
<xml_diff>
--- a/Exercises 1.xlsx
+++ b/Exercises 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepoIMR\BelajarExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26D590F-FADE-424F-916F-171508032613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C721A93-D504-4D83-9406-382E30AA7328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{D55AD04E-A305-41EC-8AE6-4ADCE0DCACFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="6" activeTab="12" xr2:uid="{D55AD04E-A305-41EC-8AE6-4ADCE0DCACFC}"/>
   </bookViews>
   <sheets>
     <sheet name="RUMUS" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,14 @@
     <sheet name="LATIHAN 2" sheetId="3" r:id="rId3"/>
     <sheet name="LATIHAN 3" sheetId="4" r:id="rId4"/>
     <sheet name="LATIHAN 4" sheetId="5" r:id="rId5"/>
+    <sheet name="LATIHAN 5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
+    <sheet name="LATIHAN 6" sheetId="8" r:id="rId8"/>
+    <sheet name="LATIHAN 7" sheetId="9" r:id="rId9"/>
+    <sheet name="LATIHAN 8" sheetId="10" r:id="rId10"/>
+    <sheet name="LATIHAN 9" sheetId="11" r:id="rId11"/>
+    <sheet name="LATIHAN 10" sheetId="12" r:id="rId12"/>
+    <sheet name="LATIHAN 11" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="198">
   <si>
     <t>no</t>
   </si>
@@ -115,9 +123,6 @@
     <t>hlookup</t>
   </si>
   <si>
-    <t>bonus rumus:iferror</t>
-  </si>
-  <si>
     <t>bagian 1</t>
   </si>
   <si>
@@ -310,10 +315,322 @@
     <t>mengambil data dari karakter tertentu menggunakan rumus left, mid, dan right</t>
   </si>
   <si>
-    <t xml:space="preserve">nilai </t>
-  </si>
-  <si>
-    <t>hasil</t>
+    <t>Nama Murid</t>
+  </si>
+  <si>
+    <t>pembulatan kebawah</t>
+  </si>
+  <si>
+    <t>pembulatan ke atas</t>
+  </si>
+  <si>
+    <t>pembulatan terdekat</t>
+  </si>
+  <si>
+    <t>Andi</t>
+  </si>
+  <si>
+    <t>Budi</t>
+  </si>
+  <si>
+    <t>Rudi</t>
+  </si>
+  <si>
+    <t>Anggi</t>
+  </si>
+  <si>
+    <t>Sanadi</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>shampo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sabun </t>
+  </si>
+  <si>
+    <t>diterjen</t>
+  </si>
+  <si>
+    <t>sarden</t>
+  </si>
+  <si>
+    <t>bearbrand</t>
+  </si>
+  <si>
+    <t>stok (pcs) bil int</t>
+  </si>
+  <si>
+    <t>bil float decimal</t>
+  </si>
+  <si>
+    <t>pembulatan nilai jika di belakang koma tidak ingin ada nilai maka menggunakan rumus roundup pembulatannya akan ke atas atau +1</t>
+  </si>
+  <si>
+    <t>pembulatan nilai jika di belakgan koma tidak ingin ada nilai menggunakan rumus rounddown pembulatannya kebawah atau -1</t>
+  </si>
+  <si>
+    <t>Santi</t>
+  </si>
+  <si>
+    <t>rumus round untuk membulatkan angka sesuai dengan aturan matematika biasa. Jika angka desimal lebih dari atau sama dengan 5, maka angka bulat yang lebih tinggi akan dihasilkan; jika kurang dari 5, maka angka bulat yang lebih rendah dihasilkan.</t>
+  </si>
+  <si>
+    <t>Fungsi FLOOR digunakan untuk membulatkan angka ke bilangan bulat terbesar yang kurang dari atau sama dengan angka yang diberikan.</t>
+  </si>
+  <si>
+    <t>Fungsi CEILING digunakan untuk membulatkan angka ke bilangan bulat terkecil yang lebih besar dari atau sama dengan angka yang diberikan.</t>
+  </si>
+  <si>
+    <t>Fungsi MROUND digunakan untuk membulatkan angka ke kelipatan tertentu yang Anda tentukan.</t>
+  </si>
+  <si>
+    <t>tanggal pemesanan</t>
+  </si>
+  <si>
+    <t>no pemesanan</t>
+  </si>
+  <si>
+    <t>nama customer</t>
+  </si>
+  <si>
+    <t>domisili</t>
+  </si>
+  <si>
+    <t>lama pengiriman</t>
+  </si>
+  <si>
+    <t>iferror</t>
+  </si>
+  <si>
+    <t>RUMUS</t>
+  </si>
+  <si>
+    <t>jenis kel</t>
+  </si>
+  <si>
+    <t>toni</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bandung </t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Banten</t>
+  </si>
+  <si>
+    <t>Kalimantan</t>
+  </si>
+  <si>
+    <t>Tanggerang</t>
+  </si>
+  <si>
+    <t>Surabaya</t>
+  </si>
+  <si>
+    <t>Yogyakarta</t>
+  </si>
+  <si>
+    <t>nama murid</t>
+  </si>
+  <si>
+    <t>jenis kelamin</t>
+  </si>
+  <si>
+    <t>bil random</t>
+  </si>
+  <si>
+    <t>andi</t>
+  </si>
+  <si>
+    <t>budi</t>
+  </si>
+  <si>
+    <t>dono</t>
+  </si>
+  <si>
+    <t>kasino</t>
+  </si>
+  <si>
+    <t>indro</t>
+  </si>
+  <si>
+    <t>odang</t>
+  </si>
+  <si>
+    <t>subagjo</t>
+  </si>
+  <si>
+    <t>bejo</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>randbetween</t>
+  </si>
+  <si>
+    <t>untuk menampilkan bilangan random</t>
+  </si>
+  <si>
+    <t>untuk menampilkan bil random dengan menentukan batas bawah dan batas atas</t>
+  </si>
+  <si>
+    <t>Nama buah</t>
+  </si>
+  <si>
+    <t>Harga</t>
+  </si>
+  <si>
+    <t>Stok</t>
+  </si>
+  <si>
+    <t>Cek stok</t>
+  </si>
+  <si>
+    <t>stok</t>
+  </si>
+  <si>
+    <t>Jambu</t>
+  </si>
+  <si>
+    <t>Apel</t>
+  </si>
+  <si>
+    <t>Sawo</t>
+  </si>
+  <si>
+    <t>Mangga</t>
+  </si>
+  <si>
+    <t>Melon</t>
+  </si>
+  <si>
+    <t>Manggis</t>
+  </si>
+  <si>
+    <t>Nangka</t>
+  </si>
+  <si>
+    <t>Semangka</t>
+  </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>tanggal lahir</t>
+  </si>
+  <si>
+    <t>umur</t>
+  </si>
+  <si>
+    <t>sanadi</t>
+  </si>
+  <si>
+    <t>suwandi</t>
+  </si>
+  <si>
+    <t>santi</t>
+  </si>
+  <si>
+    <t>indri</t>
+  </si>
+  <si>
+    <t>edi</t>
+  </si>
+  <si>
+    <t>untuk menghitung umur</t>
+  </si>
+  <si>
+    <t>DATEDIF(B2,TODAY(),"y")</t>
+  </si>
+  <si>
+    <t>tanggal awal</t>
+  </si>
+  <si>
+    <t>tanggal akhir</t>
+  </si>
+  <si>
+    <t>hari libur</t>
+  </si>
+  <si>
+    <t>hari kerja</t>
+  </si>
+  <si>
+    <t>Rumus</t>
+  </si>
+  <si>
+    <t>NETWORKDAYS(C5,D5,C9)</t>
+  </si>
+  <si>
+    <t>untuk menentukan hari kerja beserta hari libur</t>
+  </si>
+  <si>
+    <t>jenkel</t>
+  </si>
+  <si>
+    <t>skor</t>
+  </si>
+  <si>
+    <t>nilai</t>
+  </si>
+  <si>
+    <t>nilai akhir</t>
+  </si>
+  <si>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>51-70</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>71-90</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>91-100</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>untuk menentukan kondisi nilai</t>
+  </si>
+  <si>
+    <t>cara 1</t>
+  </si>
+  <si>
+    <t>cara 2</t>
+  </si>
+  <si>
+    <t>cara 3</t>
+  </si>
+  <si>
+    <t>cara 4</t>
+  </si>
+  <si>
+    <t>cara 5</t>
+  </si>
+  <si>
+    <t>CARA MENAMBAHKAN NO URUT DENGAN MENGGUNAKAN 5 CARA</t>
   </si>
 </sst>
 </file>
@@ -371,7 +688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -431,18 +748,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,16 +812,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -788,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55F799E-6A89-45AD-9A0A-51C21701D1D6}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,8 +1160,8 @@
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
+      <c r="C2" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,57 +1169,57 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="25"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>30</v>
+      <c r="C10" s="26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,29 +1227,29 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="27"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="28"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>31</v>
+      <c r="C14" s="26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,36 +1257,36 @@
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="27"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="27"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="27"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>32</v>
+      <c r="C19" s="26" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,43 +1294,43 @@
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="27"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="27"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="27"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>33</v>
+      <c r="C25" s="26" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,20 +1338,20 @@
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="10"/>
+        <v>121</v>
+      </c>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="C28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1019,12 +1366,746 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC892AD-A44E-4B81-8946-E7516D116F33}">
+  <dimension ref="B5:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="22">
+        <v>36526</v>
+      </c>
+      <c r="D6" s="3">
+        <f ca="1">DATEDIF(C6,TODAY(),"y")</f>
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="22">
+        <v>37317</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ref="D7:D12" ca="1" si="0">DATEDIF(C7,TODAY(),"y")</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="22">
+        <v>36257</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="22">
+        <v>35558</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="22">
+        <v>34951</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="22">
+        <v>32914</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="22">
+        <v>37289</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B95FF8F-D26D-41B4-BD21-813C84170B74}">
+  <dimension ref="C4:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="18">
+        <v>45181</v>
+      </c>
+      <c r="D5" s="18">
+        <v>45212</v>
+      </c>
+      <c r="E5" s="3">
+        <f>NETWORKDAYS(C5,D5)</f>
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="18">
+        <v>45181</v>
+      </c>
+      <c r="D6" s="18">
+        <v>45219</v>
+      </c>
+      <c r="E6" s="3">
+        <f>NETWORKDAYS(C6,D6)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="18">
+        <v>45245</v>
+      </c>
+      <c r="D7" s="18">
+        <v>45280</v>
+      </c>
+      <c r="E7" s="3">
+        <f>NETWORKDAYS(C7,D7)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="18">
+        <v>45240</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="18">
+        <v>45274</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC39298F-D21C-4780-BEE8-E73DC05BCE96}">
+  <dimension ref="C4:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>IF(E5&gt;90,"Nilainya A",IF(E5&gt;70,"Nilainya B",IF(E5&gt;50,"Nilainya C","Nilainya D")))</f>
+        <v>Nilainya B</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3">
+        <v>74</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" ref="F6:F11" si="0">IF(E6&gt;90,"Nilainya A",IF(E6&gt;70,"Nilainya B",IF(E6&gt;50,"Nilainya C","Nilainya D")))</f>
+        <v>Nilainya B</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3">
+        <v>88</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Nilainya B</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Nilainya D</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3">
+        <v>75</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Nilainya B</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3">
+        <v>92</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Nilainya A</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3">
+        <v>95</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Nilainya A</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835654A2-14F5-437D-96E3-659BD1271BFD}">
+  <dimension ref="B2:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+      <c r="D6" s="32">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="e">
+        <f ca="1">SEQUENCE(1000)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G6">
+        <f>ROW()-1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="32">
+        <v>2</v>
+      </c>
+      <c r="D7" s="32">
+        <f>D6+1</f>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G25" si="0">ROW()-1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="32">
+        <v>3</v>
+      </c>
+      <c r="D8" s="32">
+        <f t="shared" ref="D8:D20" si="1">D7+1</f>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="32">
+        <v>4</v>
+      </c>
+      <c r="D9" s="32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="32">
+        <v>5</v>
+      </c>
+      <c r="D10" s="32">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="32">
+        <v>6</v>
+      </c>
+      <c r="D11" s="32">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="32">
+        <v>7</v>
+      </c>
+      <c r="D12" s="32">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="32">
+        <v>8</v>
+      </c>
+      <c r="D13" s="32">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="32">
+        <v>9</v>
+      </c>
+      <c r="D14" s="32">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="32">
+        <v>10</v>
+      </c>
+      <c r="D15" s="32">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="32">
+        <v>11</v>
+      </c>
+      <c r="D16" s="32">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="32">
+        <v>12</v>
+      </c>
+      <c r="D17" s="32">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="32">
+        <v>13</v>
+      </c>
+      <c r="D18" s="32">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="32">
+        <v>14</v>
+      </c>
+      <c r="D19" s="32">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="32">
+        <v>15</v>
+      </c>
+      <c r="D20" s="32">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166CB0A0-EF48-4031-AED5-FAC05EBC848D}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,31 +2118,31 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
@@ -1069,10 +2150,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5">
         <v>5000000</v>
@@ -1100,15 +2181,15 @@
         <v>3</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="5">
         <v>7000000</v>
@@ -1128,11 +2209,11 @@
         <v>6666666.666666667</v>
       </c>
       <c r="H3" s="3" t="str">
-        <f t="shared" ref="H3:H7" si="2">IF(F3&gt;20000000,"Lulus","Gagal")</f>
+        <f t="shared" ref="H3:H6" si="2">IF(F3&gt;20000000,"Lulus","Gagal")</f>
         <v>Gagal</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I7" si="3">RANK(F3,$F$3:$F$6)</f>
+        <f t="shared" ref="I3:I6" si="3">RANK(F3,$F$3:$F$6)</f>
         <v>3</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -1141,10 +2222,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5">
         <v>4000000</v>
@@ -1177,10 +2258,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5">
         <v>8000000</v>
@@ -1213,10 +2294,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C6" s="5">
         <v>9000000</v>
@@ -1248,49 +2329,43 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="L7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6">
         <f>SUM(F2:F6)</f>
         <v>102000000</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="A9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6">
         <f>AVERAGE(F2:F6)</f>
         <v>20400000</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" t="str">
         <f>IF(F2&gt;20000000,"Lulus","Tidak mencapai target")</f>
@@ -1299,7 +2374,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <f>RANK(F2,$F$3:$F$6)</f>
@@ -1308,7 +2383,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="3">
         <f>COUNT(C2:C6)</f>
@@ -1321,34 +2396,34 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="12">
+        <v>55</v>
+      </c>
+      <c r="F13" s="6">
         <f>MAX(F2:F6)</f>
         <v>24000000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="12">
+        <v>56</v>
+      </c>
+      <c r="F14" s="6">
         <f>MIN(F2:F6)</f>
         <v>16000000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="18">
+        <v>58</v>
+      </c>
+      <c r="F15" s="10">
         <f>SUMIF(B2:B6,"l",F2:F6)</f>
         <v>82000000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16">
         <f>COUNTIF(H2:H6,"lulus")</f>
@@ -1366,7 +2441,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +2451,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1386,11 +2461,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="3" t="s">
         <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -1398,10 +2473,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>13</v>
@@ -1409,7 +2484,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="str">
         <f>TRIM(B4)</f>
@@ -1421,7 +2496,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3" t="str">
         <f>LOWER(B5)</f>
@@ -1430,7 +2505,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3" t="str">
         <f>UPPER(B6)</f>
@@ -1439,7 +2514,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="str">
         <f>PROPER(B7)</f>
@@ -1448,22 +2523,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1489,31 +2564,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3">
         <v>1992</v>
@@ -1532,10 +2607,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3">
         <v>1999</v>
@@ -1554,10 +2629,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="3">
         <v>2001</v>
@@ -1576,10 +2651,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="3">
         <v>20002</v>
@@ -1602,25 +2677,25 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3">
         <v>8179187676</v>
@@ -1640,7 +2715,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3">
         <v>8179187677</v>
@@ -1660,7 +2735,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="3">
         <v>8179187678</v>
@@ -1680,7 +2755,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="3">
         <v>8179187679</v>
@@ -1700,17 +2775,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1720,79 +2795,1012 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F73736-1B24-4799-B2F8-E0FADC570BB6}">
-  <dimension ref="D3:K9"/>
+  <dimension ref="A3:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="20" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="G3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="21">
-        <v>7456789</v>
-      </c>
-      <c r="E4" s="3">
-        <f>ROUNDDOWN(D4,2)</f>
-        <v>7456789</v>
-      </c>
-      <c r="K4" s="2" t="s">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="16">
+        <v>80.22</v>
+      </c>
+      <c r="E4" s="13">
+        <f>ROUNDDOWN(D4,0)</f>
+        <v>80</v>
+      </c>
+      <c r="F4" s="13">
+        <f>ROUNDUP(D4,0)</f>
+        <v>81</v>
+      </c>
+      <c r="G4" s="13">
+        <f>ROUND(D4,0)</f>
+        <v>80</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="21">
-        <v>7456789</v>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="16">
+        <v>48.84</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" ref="E5:E9" si="0">ROUNDDOWN(D5,0)</f>
+        <v>48</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" ref="F5:F8" si="1">ROUNDUP(D5,0)</f>
+        <v>49</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" ref="G5:G8" si="2">ROUND(D5,0)</f>
+        <v>49</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="16">
+        <v>75.319999999999993</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="16">
+        <v>44.44</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="16">
+        <v>7.65</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="16">
+        <v>75.819999999999993</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" ref="F9" si="3">ROUNDUP(D9,0)</f>
+        <v>76</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" ref="G9" si="4">ROUND(D9,0)</f>
+        <v>76</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="17">
+        <v>1140</v>
+      </c>
+      <c r="E12" s="3">
+        <f>FLOOR(D12,100)</f>
+        <v>1100</v>
+      </c>
+      <c r="F12" s="3">
+        <f>CEILING(D12,100)</f>
+        <v>1200</v>
+      </c>
+      <c r="G12" s="3">
+        <f>MROUND(D12,100)</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="15">
+        <v>540</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13:E16" si="5">FLOOR(D13,100)</f>
+        <v>500</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ref="F13:F16" si="6">CEILING(D13,100)</f>
+        <v>600</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" ref="G13:G16" si="7">MROUND(D13,100)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="15">
+        <v>320</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="15">
+        <v>400</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="7"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="15">
+        <v>240</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="6"/>
+        <v>300</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="7"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BF82D9-FE3C-4B78-AC14-3F337EBBEC49}">
+  <dimension ref="B3:O10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
+        <v>45203</v>
+      </c>
+      <c r="C4" s="3">
+        <v>102</v>
+      </c>
+      <c r="D4" s="19" t="str">
+        <f>VLOOKUP(C4,$L$3:$O$11,2,0)</f>
+        <v>Andi</v>
+      </c>
+      <c r="E4" s="3" t="e">
+        <f>v</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="3">
+        <v>102</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>45201</v>
+      </c>
+      <c r="C5" s="3">
+        <v>48</v>
+      </c>
+      <c r="D5" s="19" t="str">
+        <f t="shared" ref="D5:D10" si="0">VLOOKUP(C5,$L$3:$O$11,2,0)</f>
+        <v>Budi</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="K5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="21">
-        <v>7456789</v>
+      <c r="F5" s="3"/>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="3">
+        <v>48</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>45202</v>
+      </c>
+      <c r="C6" s="3">
+        <v>55</v>
+      </c>
+      <c r="D6" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Rudi</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="K6" s="2" t="s">
+      <c r="F6" s="3"/>
+      <c r="H6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="3">
+        <v>55</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>45209</v>
+      </c>
+      <c r="C7" s="3">
+        <v>80</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Anggi</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="L7" s="3">
+        <v>80</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>45212</v>
+      </c>
+      <c r="C8" s="3">
+        <v>72</v>
+      </c>
+      <c r="D8" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Sanadi</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="L8" s="3">
+        <v>72</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>45217</v>
+      </c>
+      <c r="C9" s="3">
+        <v>88</v>
+      </c>
+      <c r="D9" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Santi</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="L9" s="3">
+        <v>88</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>45204</v>
+      </c>
+      <c r="C10" s="3">
+        <v>99</v>
+      </c>
+      <c r="D10" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>toni</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="L10" s="3">
+        <v>99</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F94CA-DD39-42D3-9B21-19B29D422476}">
+  <dimension ref="D5:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <v>102</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>80</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>88</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>99</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8391B486-3721-4CA5-B25D-95534EF8E9D1}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="3">
+        <f ca="1">RAND()</f>
+        <v>0.23287300673657874</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D10" ca="1" si="0">RAND()</f>
+        <v>0.37371607824612763</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17354578290777323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.87794321261422048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55825065994681367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46342630982220745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25947163755670111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.77868626566597332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.5682814877623978E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE9A4C4-F31A-4A60-A3D5-228E1C699ED8}">
+  <dimension ref="C4:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="13">
+        <v>6000</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="3">
+        <f>IFERROR(VLOOKUP(G5,$C$4:$E$9,3,0),"Stok Tidak Ada!")</f>
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D7" s="21">
-        <v>7456789</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="K7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D8" s="21">
-        <v>7456789</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="K8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K9" s="2" t="s">
-        <v>25</v>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="13">
+        <v>8500</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="3">
+        <f>IFERROR(VLOOKUP(G6,$C$4:$E$9,3,0),"Stok Tidak Ada!")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="13">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f>IFERROR(VLOOKUP(G7,$C$4:$E$9,3,0),"Stok Tidak Ada!")</f>
+        <v>Stok Tidak Ada!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="13">
+        <v>4000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f>IFERROR(VLOOKUP(G8,$C$4:$E$9,3,0),"Stok Tidak Ada!")</f>
+        <v>Stok Tidak Ada!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="13">
+        <v>5000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f>IFERROR(VLOOKUP(G9,$C$4:$E$9,3,0),"Stok Tidak Ada!")</f>
+        <v>Stok Tidak Ada!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>